<commit_message>
Resolução do problema de duplicação de linhas
</commit_message>
<xml_diff>
--- a/tabela_imprimir.xlsx
+++ b/tabela_imprimir.xlsx
@@ -441,7 +441,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="10" customWidth="1" min="1" max="1"/>
-    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="6" customWidth="1" min="2" max="2"/>
     <col width="30" customWidth="1" min="3" max="3"/>
     <col width="5" customWidth="1" min="4" max="4"/>
     <col width="5" customWidth="1" min="5" max="5"/>
@@ -459,7 +459,7 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>Deriv_x</t>
+          <t>Deriv</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
@@ -502,7 +502,7 @@
       <c r="A2" s="3" t="n">
         <v>160002006</v>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>3000</t>
         </is>
@@ -512,22 +512,22 @@
           <t xml:space="preserve">BUCHA 8MM (PAREDE) NEUTRO     </t>
         </is>
       </c>
-      <c r="D2" s="3" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>R3E</t>
         </is>
       </c>
-      <c r="E2" s="3" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>S2</t>
         </is>
       </c>
-      <c r="F2" s="3" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>D0</t>
         </is>
       </c>
-      <c r="G2" s="3" t="inlineStr">
+      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>8.000,00</t>
         </is>
@@ -547,7 +547,7 @@
       <c r="A3" s="3" t="n">
         <v>160006011</v>
       </c>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -557,22 +557,22 @@
           <t>PREGO 8X8 COM CABECA LISO - 18</t>
         </is>
       </c>
-      <c r="D3" s="3" t="inlineStr">
+      <c r="D3" s="2" t="inlineStr">
         <is>
           <t>R3E</t>
         </is>
       </c>
-      <c r="E3" s="3" t="inlineStr">
+      <c r="E3" s="2" t="inlineStr">
         <is>
           <t>S3</t>
         </is>
       </c>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="F3" s="2" t="inlineStr">
         <is>
           <t>D0</t>
         </is>
       </c>
-      <c r="G3" s="3" t="inlineStr">
+      <c r="G3" s="2" t="inlineStr">
         <is>
           <t>200.000,00</t>
         </is>
@@ -588,7 +588,7 @@
       <c r="A4" s="3" t="n">
         <v>160006018</v>
       </c>
-      <c r="B4" s="3" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -598,22 +598,22 @@
           <t>PARAFUSO 4,5X22 CABECA CHATA -</t>
         </is>
       </c>
-      <c r="D4" s="3" t="inlineStr">
+      <c r="D4" s="2" t="inlineStr">
         <is>
           <t>R3E</t>
         </is>
       </c>
-      <c r="E4" s="3" t="inlineStr">
+      <c r="E4" s="2" t="inlineStr">
         <is>
           <t>S3</t>
         </is>
       </c>
-      <c r="F4" s="3" t="inlineStr">
+      <c r="F4" s="2" t="inlineStr">
         <is>
           <t>D1</t>
         </is>
       </c>
-      <c r="G4" s="3" t="inlineStr">
+      <c r="G4" s="2" t="inlineStr">
         <is>
           <t>40.000,00</t>
         </is>
@@ -629,7 +629,7 @@
       <c r="A5" s="3" t="n">
         <v>160006016</v>
       </c>
-      <c r="B5" s="3" t="inlineStr">
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -639,22 +639,22 @@
           <t>PARAFUSO 3,5X12 CABECA FLANGEA</t>
         </is>
       </c>
-      <c r="D5" s="3" t="inlineStr">
+      <c r="D5" s="2" t="inlineStr">
         <is>
           <t>R3E</t>
         </is>
       </c>
-      <c r="E5" s="3" t="inlineStr">
+      <c r="E5" s="2" t="inlineStr">
         <is>
           <t>S4</t>
         </is>
       </c>
-      <c r="F5" s="3" t="inlineStr">
+      <c r="F5" s="2" t="inlineStr">
         <is>
           <t>E1</t>
         </is>
       </c>
-      <c r="G5" s="3" t="inlineStr">
+      <c r="G5" s="2" t="inlineStr">
         <is>
           <t>260.000,00</t>
         </is>
@@ -670,7 +670,7 @@
       <c r="A6" s="3" t="n">
         <v>160006016</v>
       </c>
-      <c r="B6" s="3" t="inlineStr">
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -680,22 +680,22 @@
           <t>PARAFUSO 3,5X12 CABECA FLANGEA</t>
         </is>
       </c>
-      <c r="D6" s="3" t="inlineStr">
+      <c r="D6" s="2" t="inlineStr">
         <is>
           <t>R3E</t>
         </is>
       </c>
-      <c r="E6" s="3" t="inlineStr">
+      <c r="E6" s="2" t="inlineStr">
         <is>
           <t>S4</t>
         </is>
       </c>
-      <c r="F6" s="3" t="inlineStr">
+      <c r="F6" s="2" t="inlineStr">
         <is>
           <t>E0</t>
         </is>
       </c>
-      <c r="G6" s="3" t="inlineStr">
+      <c r="G6" s="2" t="inlineStr">
         <is>
           <t>260.000,00</t>
         </is>
@@ -711,7 +711,7 @@
       <c r="A7" s="3" t="n">
         <v>160006010</v>
       </c>
-      <c r="B7" s="3" t="inlineStr">
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -721,22 +721,22 @@
           <t>PARAFUSO 4,5X50 CABECA CHATA P</t>
         </is>
       </c>
-      <c r="D7" s="3" t="inlineStr">
+      <c r="D7" s="2" t="inlineStr">
         <is>
           <t>R3E</t>
         </is>
       </c>
-      <c r="E7" s="3" t="inlineStr">
+      <c r="E7" s="2" t="inlineStr">
         <is>
           <t>S5</t>
         </is>
       </c>
-      <c r="F7" s="3" t="inlineStr">
+      <c r="F7" s="2" t="inlineStr">
         <is>
           <t>D0</t>
         </is>
       </c>
-      <c r="G7" s="3" t="inlineStr">
+      <c r="G7" s="2" t="inlineStr">
         <is>
           <t>12.000,00</t>
         </is>
@@ -752,7 +752,7 @@
       <c r="A8" s="3" t="n">
         <v>160001034</v>
       </c>
-      <c r="B8" s="3" t="inlineStr">
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -762,22 +762,22 @@
           <t>CHAPA JUNCAO 18X40 COM 2 FUROS</t>
         </is>
       </c>
-      <c r="D8" s="3" t="inlineStr">
+      <c r="D8" s="2" t="inlineStr">
         <is>
           <t>R3E</t>
         </is>
       </c>
-      <c r="E8" s="3" t="inlineStr">
+      <c r="E8" s="2" t="inlineStr">
         <is>
           <t>S7</t>
         </is>
       </c>
-      <c r="F8" s="3" t="inlineStr">
+      <c r="F8" s="2" t="inlineStr">
         <is>
           <t>E0</t>
         </is>
       </c>
-      <c r="G8" s="3" t="inlineStr">
+      <c r="G8" s="2" t="inlineStr">
         <is>
           <t>10.000,00</t>
         </is>
@@ -793,7 +793,7 @@
       <c r="A9" s="3" t="n">
         <v>160001034</v>
       </c>
-      <c r="B9" s="3" t="inlineStr">
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -803,22 +803,22 @@
           <t>CHAPA JUNCAO 18X40 COM 2 FUROS</t>
         </is>
       </c>
-      <c r="D9" s="3" t="inlineStr">
+      <c r="D9" s="2" t="inlineStr">
         <is>
           <t>R3E</t>
         </is>
       </c>
-      <c r="E9" s="3" t="inlineStr">
+      <c r="E9" s="2" t="inlineStr">
         <is>
           <t>S7</t>
         </is>
       </c>
-      <c r="F9" s="3" t="inlineStr">
+      <c r="F9" s="2" t="inlineStr">
         <is>
           <t>D0</t>
         </is>
       </c>
-      <c r="G9" s="3" t="inlineStr">
+      <c r="G9" s="2" t="inlineStr">
         <is>
           <t>10.000,00</t>
         </is>
@@ -834,7 +834,7 @@
       <c r="A10" s="3" t="n">
         <v>160001032</v>
       </c>
-      <c r="B10" s="3" t="inlineStr">
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -844,22 +844,22 @@
           <t>CANTONEIRA PLASTICA CINZA 20X2</t>
         </is>
       </c>
-      <c r="D10" s="3" t="inlineStr">
+      <c r="D10" s="2" t="inlineStr">
         <is>
           <t>R3E</t>
         </is>
       </c>
-      <c r="E10" s="3" t="inlineStr">
+      <c r="E10" s="2" t="inlineStr">
         <is>
           <t>S7</t>
         </is>
       </c>
-      <c r="F10" s="3" t="inlineStr">
+      <c r="F10" s="2" t="inlineStr">
         <is>
           <t>E1</t>
         </is>
       </c>
-      <c r="G10" s="3" t="inlineStr">
+      <c r="G10" s="2" t="inlineStr">
         <is>
           <t>10.000,00</t>
         </is>
@@ -875,7 +875,7 @@
       <c r="A11" s="3" t="n">
         <v>160001011</v>
       </c>
-      <c r="B11" s="3" t="inlineStr">
+      <c r="B11" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -885,22 +885,22 @@
           <t>SUPORTE ANGULAR CENTRAL MARRON</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
+      <c r="D11" s="2" t="inlineStr">
         <is>
           <t>R3E</t>
         </is>
       </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="E11" s="2" t="inlineStr">
         <is>
           <t>S8</t>
         </is>
       </c>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="F11" s="2" t="inlineStr">
         <is>
           <t>D2</t>
         </is>
       </c>
-      <c r="G11" s="3" t="inlineStr">
+      <c r="G11" s="2" t="inlineStr">
         <is>
           <t>10.000,00</t>
         </is>
@@ -916,7 +916,7 @@
       <c r="A12" s="3" t="n">
         <v>160001024</v>
       </c>
-      <c r="B12" s="3" t="inlineStr">
+      <c r="B12" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -926,22 +926,22 @@
           <t>PINO GIROFIX COM ROSCA SOBERBA</t>
         </is>
       </c>
-      <c r="D12" s="3" t="inlineStr">
+      <c r="D12" s="2" t="inlineStr">
         <is>
           <t>R3E</t>
         </is>
       </c>
-      <c r="E12" s="3" t="inlineStr">
+      <c r="E12" s="2" t="inlineStr">
         <is>
           <t>S8</t>
         </is>
       </c>
-      <c r="F12" s="3" t="inlineStr">
+      <c r="F12" s="2" t="inlineStr">
         <is>
           <t>E0</t>
         </is>
       </c>
-      <c r="G12" s="3" t="inlineStr">
+      <c r="G12" s="2" t="inlineStr">
         <is>
           <t>50.000,00</t>
         </is>
@@ -957,7 +957,7 @@
       <c r="A13" s="3" t="n">
         <v>160001024</v>
       </c>
-      <c r="B13" s="3" t="inlineStr">
+      <c r="B13" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -967,22 +967,22 @@
           <t>PINO GIROFIX COM ROSCA SOBERBA</t>
         </is>
       </c>
-      <c r="D13" s="3" t="inlineStr">
+      <c r="D13" s="2" t="inlineStr">
         <is>
           <t>R3E</t>
         </is>
       </c>
-      <c r="E13" s="3" t="inlineStr">
+      <c r="E13" s="2" t="inlineStr">
         <is>
           <t>S8</t>
         </is>
       </c>
-      <c r="F13" s="3" t="inlineStr">
+      <c r="F13" s="2" t="inlineStr">
         <is>
           <t>D0</t>
         </is>
       </c>
-      <c r="G13" s="3" t="inlineStr">
+      <c r="G13" s="2" t="inlineStr">
         <is>
           <t>50.000,00</t>
         </is>
@@ -998,7 +998,7 @@
       <c r="A14" s="3" t="n">
         <v>160002003</v>
       </c>
-      <c r="B14" s="3" t="inlineStr">
+      <c r="B14" s="2" t="inlineStr">
         <is>
           <t>3014</t>
         </is>
@@ -1008,22 +1008,22 @@
           <t>SUPORTE PRATELEIRA NYLON 8X10M</t>
         </is>
       </c>
-      <c r="D14" s="3" t="inlineStr">
+      <c r="D14" s="2" t="inlineStr">
         <is>
           <t>R3E</t>
         </is>
       </c>
-      <c r="E14" s="3" t="inlineStr">
+      <c r="E14" s="2" t="inlineStr">
         <is>
           <t>S9</t>
         </is>
       </c>
-      <c r="F14" s="3" t="inlineStr">
+      <c r="F14" s="2" t="inlineStr">
         <is>
           <t>E2</t>
         </is>
       </c>
-      <c r="G14" s="3" t="inlineStr">
+      <c r="G14" s="2" t="inlineStr">
         <is>
           <t>6.000,00</t>
         </is>
@@ -1039,7 +1039,7 @@
       <c r="A15" s="3" t="n">
         <v>160001025</v>
       </c>
-      <c r="B15" s="3" t="inlineStr">
+      <c r="B15" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1049,22 +1049,22 @@
           <t>CASTANHA DO MINI-GIROFIX 12X9M</t>
         </is>
       </c>
-      <c r="D15" s="3" t="inlineStr">
+      <c r="D15" s="2" t="inlineStr">
         <is>
           <t>R3E</t>
         </is>
       </c>
-      <c r="E15" s="3" t="inlineStr">
+      <c r="E15" s="2" t="inlineStr">
         <is>
           <t>S9</t>
         </is>
       </c>
-      <c r="F15" s="3" t="inlineStr">
+      <c r="F15" s="2" t="inlineStr">
         <is>
           <t>E0</t>
         </is>
       </c>
-      <c r="G15" s="3" t="inlineStr">
+      <c r="G15" s="2" t="inlineStr">
         <is>
           <t>50.000,00</t>
         </is>
@@ -1080,7 +1080,7 @@
       <c r="A16" s="3" t="n">
         <v>160001025</v>
       </c>
-      <c r="B16" s="3" t="inlineStr">
+      <c r="B16" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1090,22 +1090,22 @@
           <t>CASTANHA DO MINI-GIROFIX 12X9M</t>
         </is>
       </c>
-      <c r="D16" s="3" t="inlineStr">
+      <c r="D16" s="2" t="inlineStr">
         <is>
           <t>R3E</t>
         </is>
       </c>
-      <c r="E16" s="3" t="inlineStr">
+      <c r="E16" s="2" t="inlineStr">
         <is>
           <t>S9</t>
         </is>
       </c>
-      <c r="F16" s="3" t="inlineStr">
+      <c r="F16" s="2" t="inlineStr">
         <is>
           <t>D0</t>
         </is>
       </c>
-      <c r="G16" s="3" t="inlineStr">
+      <c r="G16" s="2" t="inlineStr">
         <is>
           <t>50.000,00</t>
         </is>
@@ -1121,7 +1121,7 @@
       <c r="A17" s="3" t="n">
         <v>160001022</v>
       </c>
-      <c r="B17" s="3" t="inlineStr">
+      <c r="B17" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1131,10 +1131,10 @@
           <t xml:space="preserve">PORCA CILINDRICA 12X9MM       </t>
         </is>
       </c>
-      <c r="D17" s="3" t="inlineStr"/>
-      <c r="E17" s="3" t="inlineStr"/>
-      <c r="F17" s="3" t="inlineStr"/>
-      <c r="G17" s="3" t="inlineStr">
+      <c r="D17" s="2" t="inlineStr"/>
+      <c r="E17" s="2" t="inlineStr"/>
+      <c r="F17" s="2" t="inlineStr"/>
+      <c r="G17" s="2" t="inlineStr">
         <is>
           <t>6.000,00</t>
         </is>
@@ -1150,7 +1150,7 @@
       <c r="A18" s="3" t="n">
         <v>160001018</v>
       </c>
-      <c r="B18" s="3" t="inlineStr">
+      <c r="B18" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1160,10 +1160,10 @@
           <t>CANTONEIRA PLASTICA 20x20x42 C</t>
         </is>
       </c>
-      <c r="D18" s="3" t="inlineStr"/>
-      <c r="E18" s="3" t="inlineStr"/>
-      <c r="F18" s="3" t="inlineStr"/>
-      <c r="G18" s="3" t="inlineStr">
+      <c r="D18" s="2" t="inlineStr"/>
+      <c r="E18" s="2" t="inlineStr"/>
+      <c r="F18" s="2" t="inlineStr"/>
+      <c r="G18" s="2" t="inlineStr">
         <is>
           <t>33.000,00</t>
         </is>
@@ -1179,7 +1179,7 @@
       <c r="A19" s="3" t="n">
         <v>160001023</v>
       </c>
-      <c r="B19" s="3" t="inlineStr">
+      <c r="B19" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1189,10 +1189,10 @@
           <t xml:space="preserve">CAVILHA 6X30MM                </t>
         </is>
       </c>
-      <c r="D19" s="3" t="inlineStr"/>
-      <c r="E19" s="3" t="inlineStr"/>
-      <c r="F19" s="3" t="inlineStr"/>
-      <c r="G19" s="3" t="inlineStr">
+      <c r="D19" s="2" t="inlineStr"/>
+      <c r="E19" s="2" t="inlineStr"/>
+      <c r="F19" s="2" t="inlineStr"/>
+      <c r="G19" s="2" t="inlineStr">
         <is>
           <t>50.000,00</t>
         </is>
@@ -1208,7 +1208,7 @@
       <c r="A20" s="3" t="n">
         <v>170001005</v>
       </c>
-      <c r="B20" s="3" t="inlineStr">
+      <c r="B20" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1218,10 +1218,10 @@
           <t>FILME POLIETILENO (PE) 590X280</t>
         </is>
       </c>
-      <c r="D20" s="3" t="inlineStr"/>
-      <c r="E20" s="3" t="inlineStr"/>
-      <c r="F20" s="3" t="inlineStr"/>
-      <c r="G20" s="3" t="inlineStr">
+      <c r="D20" s="2" t="inlineStr"/>
+      <c r="E20" s="2" t="inlineStr"/>
+      <c r="F20" s="2" t="inlineStr"/>
+      <c r="G20" s="2" t="inlineStr">
         <is>
           <t>20,00</t>
         </is>
@@ -1237,7 +1237,7 @@
       <c r="A21" s="3" t="n">
         <v>160002012</v>
       </c>
-      <c r="B21" s="3" t="inlineStr">
+      <c r="B21" s="2" t="inlineStr">
         <is>
           <t>3039</t>
         </is>
@@ -1247,10 +1247,10 @@
           <t>GIZ DE CORRECAO 15x8 OFF WHITE</t>
         </is>
       </c>
-      <c r="D21" s="3" t="inlineStr"/>
-      <c r="E21" s="3" t="inlineStr"/>
-      <c r="F21" s="3" t="inlineStr"/>
-      <c r="G21" s="3" t="inlineStr">
+      <c r="D21" s="2" t="inlineStr"/>
+      <c r="E21" s="2" t="inlineStr"/>
+      <c r="F21" s="2" t="inlineStr"/>
+      <c r="G21" s="2" t="inlineStr">
         <is>
           <t>2.000,00</t>
         </is>
@@ -1266,7 +1266,7 @@
       <c r="A22" s="3" t="n">
         <v>160002012</v>
       </c>
-      <c r="B22" s="3" t="inlineStr">
+      <c r="B22" s="2" t="inlineStr">
         <is>
           <t>3070</t>
         </is>
@@ -1276,10 +1276,10 @@
           <t xml:space="preserve">GIZ DE CORRECAO 15x8 NATURE   </t>
         </is>
       </c>
-      <c r="D22" s="3" t="inlineStr"/>
-      <c r="E22" s="3" t="inlineStr"/>
-      <c r="F22" s="3" t="inlineStr"/>
-      <c r="G22" s="3" t="inlineStr">
+      <c r="D22" s="2" t="inlineStr"/>
+      <c r="E22" s="2" t="inlineStr"/>
+      <c r="F22" s="2" t="inlineStr"/>
+      <c r="G22" s="2" t="inlineStr">
         <is>
           <t>2.000,00</t>
         </is>
@@ -1295,7 +1295,7 @@
       <c r="A23" s="3" t="n">
         <v>160002007</v>
       </c>
-      <c r="B23" s="3" t="inlineStr">
+      <c r="B23" s="2" t="inlineStr">
         <is>
           <t>3000</t>
         </is>
@@ -1305,10 +1305,10 @@
           <t>EMBALAGEM PLASTICA VIRGEM 10X1</t>
         </is>
       </c>
-      <c r="D23" s="3" t="inlineStr"/>
-      <c r="E23" s="3" t="inlineStr"/>
-      <c r="F23" s="3" t="inlineStr"/>
-      <c r="G23" s="3" t="inlineStr">
+      <c r="D23" s="2" t="inlineStr"/>
+      <c r="E23" s="2" t="inlineStr"/>
+      <c r="F23" s="2" t="inlineStr"/>
+      <c r="G23" s="2" t="inlineStr">
         <is>
           <t>3.000,00</t>
         </is>
@@ -1324,7 +1324,7 @@
       <c r="A24" s="3" t="n">
         <v>160002002</v>
       </c>
-      <c r="B24" s="3" t="inlineStr">
+      <c r="B24" s="2" t="inlineStr">
         <is>
           <t>3070</t>
         </is>
@@ -1334,10 +1334,10 @@
           <t xml:space="preserve">TAMPA ADESIVA 18MM NATURE     </t>
         </is>
       </c>
-      <c r="D24" s="3" t="inlineStr"/>
-      <c r="E24" s="3" t="inlineStr"/>
-      <c r="F24" s="3" t="inlineStr"/>
-      <c r="G24" s="3" t="inlineStr">
+      <c r="D24" s="2" t="inlineStr"/>
+      <c r="E24" s="2" t="inlineStr"/>
+      <c r="F24" s="2" t="inlineStr"/>
+      <c r="G24" s="2" t="inlineStr">
         <is>
           <t>20.000,00</t>
         </is>
@@ -1353,7 +1353,7 @@
       <c r="A25" s="3" t="n">
         <v>160002002</v>
       </c>
-      <c r="B25" s="3" t="inlineStr">
+      <c r="B25" s="2" t="inlineStr">
         <is>
           <t>3039</t>
         </is>
@@ -1363,10 +1363,10 @@
           <t xml:space="preserve">TAMPA ADESIVA 18MM OFF WHITE  </t>
         </is>
       </c>
-      <c r="D25" s="3" t="inlineStr"/>
-      <c r="E25" s="3" t="inlineStr"/>
-      <c r="F25" s="3" t="inlineStr"/>
-      <c r="G25" s="3" t="inlineStr">
+      <c r="D25" s="2" t="inlineStr"/>
+      <c r="E25" s="2" t="inlineStr"/>
+      <c r="F25" s="2" t="inlineStr"/>
+      <c r="G25" s="2" t="inlineStr">
         <is>
           <t>40.000,00</t>
         </is>
@@ -1382,7 +1382,7 @@
       <c r="A26" s="3" t="n">
         <v>160002002</v>
       </c>
-      <c r="B26" s="3" t="inlineStr">
+      <c r="B26" s="2" t="inlineStr">
         <is>
           <t>3057</t>
         </is>
@@ -1392,10 +1392,10 @@
           <t xml:space="preserve">TAMPA ADESIVA 18MM FREIJO     </t>
         </is>
       </c>
-      <c r="D26" s="3" t="inlineStr"/>
-      <c r="E26" s="3" t="inlineStr"/>
-      <c r="F26" s="3" t="inlineStr"/>
-      <c r="G26" s="3" t="inlineStr">
+      <c r="D26" s="2" t="inlineStr"/>
+      <c r="E26" s="2" t="inlineStr"/>
+      <c r="F26" s="2" t="inlineStr"/>
+      <c r="G26" s="2" t="inlineStr">
         <is>
           <t>20.000,00</t>
         </is>
@@ -1411,7 +1411,7 @@
       <c r="A27" s="3" t="n">
         <v>310004001</v>
       </c>
-      <c r="B27" s="3" t="inlineStr">
+      <c r="B27" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1421,10 +1421,10 @@
           <t xml:space="preserve">FITA ADESIVA 48X100MM INCOLOR </t>
         </is>
       </c>
-      <c r="D27" s="3" t="inlineStr"/>
-      <c r="E27" s="3" t="inlineStr"/>
-      <c r="F27" s="3" t="inlineStr"/>
-      <c r="G27" s="3" t="inlineStr">
+      <c r="D27" s="2" t="inlineStr"/>
+      <c r="E27" s="2" t="inlineStr"/>
+      <c r="F27" s="2" t="inlineStr"/>
+      <c r="G27" s="2" t="inlineStr">
         <is>
           <t>45,00</t>
         </is>

</xml_diff>

<commit_message>
Alterações nas Logicas de Input
</commit_message>
<xml_diff>
--- a/tabela_imprimir.xlsx
+++ b/tabela_imprimir.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -47,13 +47,10 @@
       <sz val="30"/>
     </font>
     <font>
-      <sz val="60"/>
+      <sz val="150"/>
     </font>
     <font>
-      <sz val="100"/>
-    </font>
-    <font>
-      <sz val="150"/>
+      <sz val="60"/>
     </font>
     <font>
       <sz val="110"/>
@@ -142,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -165,16 +162,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -570,7 +564,7 @@
       </c>
       <c r="B2" s="10" t="inlineStr">
         <is>
-          <t>Parafuso 3,5X12 CAB FLANGEADA</t>
+          <t>CANTONEIRA PLASTICA 20x20x42</t>
         </is>
       </c>
     </row>
@@ -582,7 +576,7 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>11130585</t>
+          <t>150</t>
         </is>
       </c>
     </row>
@@ -592,9 +586,9 @@
           <t>CODIGO</t>
         </is>
       </c>
-      <c r="B4" s="12" t="inlineStr">
-        <is>
-          <t>6016</t>
+      <c r="B4" s="11" t="inlineStr">
+        <is>
+          <t>1018</t>
         </is>
       </c>
     </row>
@@ -604,7 +598,7 @@
           <t>VOL</t>
         </is>
       </c>
-      <c r="B5" s="13" t="inlineStr">
+      <c r="B5" s="12" t="inlineStr">
         <is>
           <t>10</t>
         </is>

</xml_diff>

<commit_message>
Alteração para excluir valores duplicados
</commit_message>
<xml_diff>
--- a/tabela_imprimir.xlsx
+++ b/tabela_imprimir.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,16 +495,16 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>160006021</v>
+        <v>160002006</v>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>3000</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>PARAFUSO 4,5X35 CABECA FLANGEA</t>
+          <t xml:space="preserve">BUCHA 8MM (PAREDE) NEUTRO     </t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
@@ -519,23 +519,23 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>D1</t>
+          <t>D0</t>
         </is>
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>12.000,00</t>
+          <t>8.000,00</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>177.237</t>
+          <t>177.386</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>160006011</v>
+        <v>160006015</v>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
@@ -544,7 +544,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>PREGO 8X8 COM CABECA LISO - 18</t>
+          <t>PARAFUSO 6,0X75 CABECA CHATA P</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
@@ -554,24 +554,24 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>S3</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>D0</t>
+          <t>E0</t>
         </is>
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>200.000,00</t>
+          <t>7.000,00</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>160006016</v>
+        <v>160006018</v>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
@@ -580,7 +580,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>PARAFUSO 3,5X12 CABECA FLANGEA</t>
+          <t>PARAFUSO 4,5X22 CABECA CHATA -</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
@@ -590,24 +590,24 @@
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>S4</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>E0</t>
+          <t>D1</t>
         </is>
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>100.000,00</t>
+          <t>20.000,00</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>160006016</v>
+        <v>160006011</v>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
@@ -616,7 +616,7 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>PARAFUSO 3,5X12 CABECA FLANGEA</t>
+          <t>PREGO 8X8 COM CABECA LISO - 18</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
@@ -626,33 +626,33 @@
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>S4</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
-          <t>E1</t>
+          <t>D0</t>
         </is>
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
-          <t>100.000,00</t>
+          <t>200.000,00</t>
         </is>
       </c>
       <c r="H5" s="2" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>160002004</v>
+        <v>160006008</v>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>3014</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">SAPATA OVAL 12X50 PRETO       </t>
+          <t>PARAFUSO 4,5X25 CABECA CHATA P</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
@@ -662,7 +662,7 @@
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>S6</t>
+          <t>S4</t>
         </is>
       </c>
       <c r="F6" s="2" t="inlineStr">
@@ -672,23 +672,23 @@
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>15.000,00</t>
+          <t>80.000,00</t>
         </is>
       </c>
       <c r="H6" s="2" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>160002016</v>
+        <v>160006016</v>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>3014</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">SUPORTE FIM DE CURSO 10X15 MM </t>
+          <t>PARAFUSO 3,5X12 CABECA FLANGEA</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
@@ -698,24 +698,24 @@
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>S7</t>
+          <t>S4</t>
         </is>
       </c>
       <c r="F7" s="2" t="inlineStr">
         <is>
-          <t>E1</t>
+          <t>E0</t>
         </is>
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>5.000,00</t>
+          <t>260.000,00</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>160001023</v>
+        <v>160006006</v>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
@@ -724,34 +724,34 @@
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">CAVILHA 6X30MM                </t>
+          <t>PARAFUSO 3,5X40 CABECA CHATA P</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>R3D</t>
+          <t>R3E</t>
         </is>
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>S8</t>
+          <t>S5</t>
         </is>
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>D0</t>
+          <t>E0</t>
         </is>
       </c>
       <c r="G8" s="2" t="inlineStr">
         <is>
-          <t>50.000,00</t>
+          <t>30.000,00</t>
         </is>
       </c>
       <c r="H8" s="2" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
-        <v>160001023</v>
+        <v>160006022</v>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
@@ -760,34 +760,34 @@
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">CAVILHA 6X30MM                </t>
+          <t>PARAFUSO M4 12MM CHATA PHS BIC</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>R3D</t>
+          <t>R3E</t>
         </is>
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>S8</t>
+          <t>S5</t>
         </is>
       </c>
       <c r="F9" s="2" t="inlineStr">
         <is>
-          <t>E0</t>
+          <t>D1</t>
         </is>
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>50.000,00</t>
+          <t>5.000,00</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="3" t="n">
-        <v>160001003</v>
+        <v>160001001</v>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
@@ -796,7 +796,7 @@
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">CAVILHAS 8X20MM PINUS         </t>
+          <t xml:space="preserve">COLA PARA MONTAGEM - 08GRS    </t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
@@ -806,24 +806,24 @@
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>S8</t>
+          <t>S5</t>
         </is>
       </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
-          <t>D1</t>
+          <t>E1</t>
         </is>
       </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
-          <t>20.000,00</t>
+          <t>1.000,00</t>
         </is>
       </c>
       <c r="H10" s="2" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="3" t="n">
-        <v>160001011</v>
+        <v>160006010</v>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
@@ -832,7 +832,7 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>SUPORTE ANGULAR CENTRAL MARRON</t>
+          <t>PARAFUSO 4,5X50 CABECA CHATA P</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
@@ -842,24 +842,24 @@
       </c>
       <c r="E11" s="2" t="inlineStr">
         <is>
-          <t>S8</t>
+          <t>S5</t>
         </is>
       </c>
       <c r="F11" s="2" t="inlineStr">
         <is>
-          <t>D2</t>
+          <t>D0</t>
         </is>
       </c>
       <c r="G11" s="2" t="inlineStr">
         <is>
-          <t>30.000,00</t>
+          <t>8.000,00</t>
         </is>
       </c>
       <c r="H11" s="2" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="3" t="n">
-        <v>160001024</v>
+        <v>160006042</v>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
@@ -868,7 +868,7 @@
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>PINO GIROFIX COM ROSCA SOBERBA</t>
+          <t>PARAFUSO 3,5X30 CABECA FLANGEA</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
@@ -878,24 +878,24 @@
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>S8</t>
+          <t>S5</t>
         </is>
       </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
-          <t>D0</t>
+          <t>E3</t>
         </is>
       </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
-          <t>40.000,00</t>
+          <t>2.000,00</t>
         </is>
       </c>
       <c r="H12" s="2" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="3" t="n">
-        <v>160001024</v>
+        <v>160001032</v>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
@@ -904,7 +904,7 @@
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>PINO GIROFIX COM ROSCA SOBERBA</t>
+          <t>CANTONEIRA PLASTICA CINZA 20X2</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
@@ -914,24 +914,24 @@
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>S8</t>
+          <t>S7</t>
         </is>
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>E0</t>
+          <t>E1</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>40.000,00</t>
+          <t>4.000,00</t>
         </is>
       </c>
       <c r="H13" s="2" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="3" t="n">
-        <v>160001005</v>
+        <v>160001034</v>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
@@ -940,7 +940,7 @@
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">CAVILHA 8X55MM PINUS          </t>
+          <t>CHAPA JUNCAO 18X40 COM 2 FUROS</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr">
@@ -950,24 +950,24 @@
       </c>
       <c r="E14" s="2" t="inlineStr">
         <is>
-          <t>S8</t>
+          <t>S7</t>
         </is>
       </c>
       <c r="F14" s="2" t="inlineStr">
         <is>
-          <t>E1</t>
+          <t>E0</t>
         </is>
       </c>
       <c r="G14" s="2" t="inlineStr">
         <is>
-          <t>40,00</t>
+          <t>26.000,00</t>
         </is>
       </c>
       <c r="H14" s="2" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="3" t="n">
-        <v>160001025</v>
+        <v>160001023</v>
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
@@ -976,17 +976,17 @@
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>CASTANHA DO MINI-GIROFIX 12X9M</t>
+          <t xml:space="preserve">CAVILHA 6X30MM                </t>
         </is>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>R3E</t>
+          <t>R3D</t>
         </is>
       </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
-          <t>S9</t>
+          <t>S8</t>
         </is>
       </c>
       <c r="F15" s="2" t="inlineStr">
@@ -996,59 +996,59 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>40.000,00</t>
+          <t>100.000,00</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="3" t="n">
-        <v>160001018</v>
+        <v>160002014</v>
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>3070</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>CANTONEIRA PLASTICA 20x20x42 C</t>
+          <t>DISTANCIADOR DE PAINEL 70 X 32</t>
         </is>
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>R3D</t>
+          <t>R3E</t>
         </is>
       </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>S9</t>
+          <t>S8</t>
         </is>
       </c>
       <c r="F16" s="2" t="inlineStr">
         <is>
-          <t>E3</t>
+          <t>D3</t>
         </is>
       </c>
       <c r="G16" s="2" t="inlineStr">
         <is>
-          <t>12.000,00</t>
+          <t>1.000,00</t>
         </is>
       </c>
       <c r="H16" s="2" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="3" t="n">
-        <v>160002003</v>
+        <v>160001024</v>
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>3014</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>SUPORTE PRATELEIRA NYLON 8X10M</t>
+          <t>PINO GIROFIX COM ROSCA SOBERBA</t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr">
@@ -1058,24 +1058,24 @@
       </c>
       <c r="E17" s="2" t="inlineStr">
         <is>
-          <t>S9</t>
+          <t>S8</t>
         </is>
       </c>
       <c r="F17" s="2" t="inlineStr">
         <is>
-          <t>E2</t>
+          <t>D0</t>
         </is>
       </c>
       <c r="G17" s="2" t="inlineStr">
         <is>
-          <t>10.000,00</t>
+          <t>50.000,00</t>
         </is>
       </c>
       <c r="H17" s="2" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="3" t="n">
-        <v>160001018</v>
+        <v>160001011</v>
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
@@ -1084,34 +1084,34 @@
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>CANTONEIRA PLASTICA 20x20x42 C</t>
+          <t>SUPORTE ANGULAR CENTRAL MARRON</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>R3D</t>
+          <t>R3E</t>
         </is>
       </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>S9</t>
+          <t>S8</t>
         </is>
       </c>
       <c r="F18" s="2" t="inlineStr">
         <is>
-          <t>D0</t>
+          <t>D2</t>
         </is>
       </c>
       <c r="G18" s="2" t="inlineStr">
         <is>
-          <t>12.000,00</t>
+          <t>40.000,00</t>
         </is>
       </c>
       <c r="H18" s="2" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="3" t="n">
-        <v>160001018</v>
+        <v>160001025</v>
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
@@ -1120,12 +1120,12 @@
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>CANTONEIRA PLASTICA 20x20x42 C</t>
+          <t>CASTANHA DO MINI-GIROFIX 12X9M</t>
         </is>
       </c>
       <c r="D19" s="2" t="inlineStr">
         <is>
-          <t>R3D</t>
+          <t>R3E</t>
         </is>
       </c>
       <c r="E19" s="2" t="inlineStr">
@@ -1140,14 +1140,14 @@
       </c>
       <c r="G19" s="2" t="inlineStr">
         <is>
-          <t>12.000,00</t>
+          <t>50.000,00</t>
         </is>
       </c>
       <c r="H19" s="2" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="3" t="n">
-        <v>160001025</v>
+        <v>160001018</v>
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
@@ -1156,12 +1156,12 @@
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t>CASTANHA DO MINI-GIROFIX 12X9M</t>
+          <t>CANTONEIRA PLASTICA 20x20x42 C</t>
         </is>
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>R3E</t>
+          <t>R3D</t>
         </is>
       </c>
       <c r="E20" s="2" t="inlineStr">
@@ -1171,52 +1171,64 @@
       </c>
       <c r="F20" s="2" t="inlineStr">
         <is>
-          <t>D0</t>
+          <t>E3</t>
         </is>
       </c>
       <c r="G20" s="2" t="inlineStr">
         <is>
-          <t>40.000,00</t>
+          <t>21.000,00</t>
         </is>
       </c>
       <c r="H20" s="2" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="3" t="n">
-        <v>160002005</v>
+        <v>160002003</v>
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>3039</t>
+          <t>3014</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>GUIA CABO / PASSA FIO 46MM +/-</t>
-        </is>
-      </c>
-      <c r="D21" s="2" t="inlineStr"/>
-      <c r="E21" s="2" t="inlineStr"/>
-      <c r="F21" s="2" t="inlineStr"/>
+          <t>SUPORTE PRATELEIRA NYLON 8X10M</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>S9</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>E2</t>
+        </is>
+      </c>
       <c r="G21" s="2" t="inlineStr">
         <is>
-          <t>2.000,00</t>
+          <t>6.000,00</t>
         </is>
       </c>
       <c r="H21" s="2" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="3" t="n">
-        <v>160002005</v>
+        <v>160002022</v>
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>3014</t>
+          <t>3039</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
         <is>
-          <t>GUIA CABO / PASSA FIO 46MM +/-</t>
+          <t xml:space="preserve">TAMPA ADESIVA 12MM OFF WHITE  </t>
         </is>
       </c>
       <c r="D22" s="2" t="inlineStr"/>
@@ -1224,7 +1236,7 @@
       <c r="F22" s="2" t="inlineStr"/>
       <c r="G22" s="2" t="inlineStr">
         <is>
-          <t>1.000,00</t>
+          <t>20.000,00</t>
         </is>
       </c>
       <c r="H22" s="2" t="inlineStr"/>
@@ -1255,16 +1267,16 @@
     </row>
     <row r="24">
       <c r="A24" s="3" t="n">
-        <v>160002012</v>
+        <v>170001005</v>
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>3070</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">GIZ DE CORRECAO 15x8 NATURE   </t>
+          <t>FILME POLIETILENO (PE) 590X280</t>
         </is>
       </c>
       <c r="D24" s="2" t="inlineStr"/>
@@ -1272,34 +1284,10 @@
       <c r="F24" s="2" t="inlineStr"/>
       <c r="G24" s="2" t="inlineStr">
         <is>
-          <t>3.000,00</t>
+          <t>40,00</t>
         </is>
       </c>
       <c r="H24" s="2" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="3" t="n">
-        <v>160002022</v>
-      </c>
-      <c r="B25" s="2" t="inlineStr">
-        <is>
-          <t>3039</t>
-        </is>
-      </c>
-      <c r="C25" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">TAMPA ADESIVA 12MM OFF WHITE  </t>
-        </is>
-      </c>
-      <c r="D25" s="2" t="inlineStr"/>
-      <c r="E25" s="2" t="inlineStr"/>
-      <c r="F25" s="2" t="inlineStr"/>
-      <c r="G25" s="2" t="inlineStr">
-        <is>
-          <t>10.000,00</t>
-        </is>
-      </c>
-      <c r="H25" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>